<commit_message>
Se actualiza el diagrama de Gantt - 22/02/2023
</commit_message>
<xml_diff>
--- a/Diagrama de Gantt - EscoArt.xlsx
+++ b/Diagrama de Gantt - EscoArt.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB305D5A-7753-4A16-8138-6DCE561052EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0333E525-4368-4C44-86DE-7D84F13D1FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="4470" windowWidth="20730" windowHeight="11760" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Púrpura" sheetId="11" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="70">
   <si>
     <t>Proyecto EscoArt</t>
   </si>
@@ -229,9 +229,6 @@
     <t>Se actualizara el diagrama de Gantt con las respectivas fechas de las actividades asignadas a los integrantes del grupo</t>
   </si>
   <si>
-    <t>Investigar APIS Seguridad</t>
-  </si>
-  <si>
     <t>Se realizara la investigacion sobre diversas apis de seguradad que se puedan aplicar al proyecto</t>
   </si>
   <si>
@@ -244,19 +241,13 @@
     <t>se debe agregar un metodo en el cual se pueda distingir en el formulario de incio de sesion si el usuario que esta ingresando es admin o usuario</t>
   </si>
   <si>
-    <t>Proceso de Facturacion</t>
-  </si>
-  <si>
-    <t>Se debe generar una factura al momento de realizar la compra con todos los datos de envio y productos seleccionados</t>
-  </si>
-  <si>
     <t>Agregar apartado de perfil de usuario para la edicion de los datos</t>
   </si>
   <si>
     <t>Agregaramos el apartado de perfil en el cual cada usuario podra ver y modificar sus datos y estos se actualizaran automaticamente en la bd</t>
   </si>
   <si>
-    <t>D A - Y B - G Q</t>
+    <t>Investigar APIS con Seguridad</t>
   </si>
 </sst>
 </file>
@@ -1390,8 +1381,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{70B51325-D3C3-4A05-BAB3-7A7400707A14}" name="Hitos" displayName="Hitos" ref="B4:J41" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="B4:J41" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{70B51325-D3C3-4A05-BAB3-7A7400707A14}" name="Hitos" displayName="Hitos" ref="B4:J40" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="B4:J40" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1686,10 +1677,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
@@ -2211,7 +2202,7 @@
         <v>51</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="E25" s="25">
         <v>45180</v>
@@ -2220,12 +2211,12 @@
         <v>45184</v>
       </c>
       <c r="G25" s="13">
-        <v>1</v>
-      </c>
-      <c r="H25" s="22" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="H25" s="22"/>
+      <c r="I25" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="I25" s="6"/>
     </row>
     <row r="26" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" outlineLevel="1">
       <c r="A26" s="3"/>
@@ -2331,51 +2322,51 @@
       <c r="I30" s="28"/>
       <c r="J30" s="24"/>
     </row>
-    <row r="31" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" outlineLevel="1">
-      <c r="A31" s="3"/>
-      <c r="B31" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C31" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E31" s="25">
-        <v>45327</v>
-      </c>
-      <c r="G31" s="13">
-        <v>0</v>
-      </c>
-      <c r="H31" s="27"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="24" t="s">
+    <row r="31" spans="1:10" ht="30" customHeight="1">
+      <c r="B31" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+    </row>
+    <row r="32" spans="1:10" ht="30" customHeight="1">
+      <c r="B32" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="25">
+        <v>45254</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="13">
+        <v>1</v>
+      </c>
+      <c r="H32" s="27" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="30" customHeight="1">
-      <c r="B32" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="24"/>
     </row>
     <row r="33" spans="2:10" ht="30" customHeight="1">
       <c r="B33" s="16" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E33" s="25">
         <v>45254</v>
@@ -2392,10 +2383,10 @@
     </row>
     <row r="34" spans="2:10" ht="30" customHeight="1">
       <c r="B34" s="16" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>19</v>
@@ -2414,57 +2405,57 @@
       <c r="J34" s="24"/>
     </row>
     <row r="35" spans="2:10" ht="30" customHeight="1">
-      <c r="B35" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35" s="26" t="s">
+      <c r="B35" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E35" s="25">
-        <v>45254</v>
-      </c>
-      <c r="F35" s="1"/>
-      <c r="G35" s="13">
-        <v>1</v>
-      </c>
-      <c r="H35" s="27" t="s">
+      <c r="C35" s="5"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="32"/>
+      <c r="J35" s="32"/>
+    </row>
+    <row r="36" spans="2:10" ht="30" customHeight="1">
+      <c r="B36" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="25">
+        <v>45327</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="H36" s="27"/>
+      <c r="I36" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="I35" s="28"/>
-      <c r="J35" s="24"/>
-    </row>
-    <row r="36" spans="2:10" ht="30" customHeight="1">
-      <c r="B36" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="32"/>
-      <c r="J36" s="32"/>
+      <c r="J36" s="24"/>
     </row>
     <row r="37" spans="2:10" ht="30" customHeight="1">
-      <c r="B37" s="16" t="s">
-        <v>66</v>
+      <c r="B37" s="36" t="s">
+        <v>67</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="E37" s="25">
         <v>45327</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="13">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="H37" s="27"/>
       <c r="I37" s="28" t="s">
@@ -2473,37 +2464,22 @@
       <c r="J37" s="24"/>
     </row>
     <row r="38" spans="2:10" ht="30" customHeight="1">
-      <c r="B38" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="C38" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E38" s="25">
-        <v>45327</v>
-      </c>
+      <c r="B38" s="16"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="25"/>
       <c r="F38" s="1"/>
-      <c r="G38" s="13">
-        <v>0</v>
-      </c>
+      <c r="G38" s="13"/>
       <c r="H38" s="27"/>
       <c r="I38" s="28"/>
-      <c r="J38" s="24" t="s">
-        <v>14</v>
-      </c>
+      <c r="J38" s="24"/>
     </row>
     <row r="39" spans="2:10" ht="30" customHeight="1">
-      <c r="B39" s="16"/>
-      <c r="C39" s="26"/>
       <c r="D39" s="7"/>
-      <c r="E39" s="25"/>
       <c r="F39" s="1"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="27"/>
-      <c r="I39" s="28"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="34"/>
+      <c r="I39" s="35"/>
       <c r="J39" s="24"/>
     </row>
     <row r="40" spans="2:10" ht="30" customHeight="1">
@@ -2513,14 +2489,6 @@
       <c r="H40" s="34"/>
       <c r="I40" s="35"/>
       <c r="J40" s="24"/>
-    </row>
-    <row r="41" spans="2:10" ht="30" customHeight="1">
-      <c r="D41" s="7"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="33"/>
-      <c r="H41" s="34"/>
-      <c r="I41" s="35"/>
-      <c r="J41" s="24"/>
     </row>
   </sheetData>
   <phoneticPr fontId="31" type="noConversion"/>
@@ -2608,7 +2576,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
+  <conditionalFormatting sqref="D31">
     <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -2622,7 +2590,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
+  <conditionalFormatting sqref="D35">
     <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -2636,7 +2604,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6:G8 G4 G15:G18 G10:G13 G20:G22 G24:G28 G30:G31">
+  <conditionalFormatting sqref="G6:G8 G4 G15:G18 G10:G13 G20:G22 G24:G28 G30">
     <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -2650,7 +2618,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G33:G35">
+  <conditionalFormatting sqref="G32:G34">
     <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -2664,7 +2632,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G37:G39">
+  <conditionalFormatting sqref="G36:G38">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -2794,7 +2762,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D32</xm:sqref>
+          <xm:sqref>D31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C367B846-96A3-4ED1-BAB5-28D2F418CDF0}">
@@ -2809,7 +2777,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D36</xm:sqref>
+          <xm:sqref>D35</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{12FE09CC-9E95-4E2A-B813-E5B1BBCC9719}">
@@ -2824,7 +2792,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G6:G8 G4 G15:G18 G10:G13 G20:G22 G24:G28 G30:G31</xm:sqref>
+          <xm:sqref>G6:G8 G4 G15:G18 G10:G13 G20:G22 G24:G28 G30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{10066124-257E-4957-ACA9-88313E4BB3CC}">
@@ -2839,7 +2807,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G33:G35</xm:sqref>
+          <xm:sqref>G32:G34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{611F804D-E1F0-45B8-9B33-E325D870EBAA}">
@@ -2854,7 +2822,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G37:G39</xm:sqref>
+          <xm:sqref>G36:G38</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2863,15 +2831,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3171,6 +3130,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3192,14 +3160,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0B0F2ED-3690-4B58-8A58-9F445988C35C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5154FCDF-22C4-473E-9895-3F25869315A8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3220,6 +3180,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0B0F2ED-3690-4B58-8A58-9F445988C35C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72214B61-5049-4980-A646-5954FFE9EB71}">
   <ds:schemaRefs>

</xml_diff>